<commit_message>
ac8 created and also saucelab-chrome driver updated
</commit_message>
<xml_diff>
--- a/credentials.xlsx
+++ b/credentials.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/values/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/values/IdeaProjects/XFleet_Cucumber/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{126C30AE-E09C-F844-9F4B-C8FDBE097FA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F8111DE-97D0-6D4F-9CF4-A85667ED8625}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8500" yWindow="4900" windowWidth="27640" windowHeight="16940" xr2:uid="{AC3FA72D-1D93-084B-BC8B-B298B3374332}"/>
+    <workbookView xWindow="-56600" yWindow="-6800" windowWidth="27640" windowHeight="16940" xr2:uid="{AC3FA72D-1D93-084B-BC8B-B298B3374332}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="155">
   <si>
     <t>Truck Driver</t>
   </si>
@@ -58,15 +58,6 @@
     <t>user32</t>
   </si>
   <si>
-    <t>user155</t>
-  </si>
-  <si>
-    <t>user174</t>
-  </si>
-  <si>
-    <t>user200</t>
-  </si>
-  <si>
     <t>storemanager51</t>
   </si>
   <si>
@@ -94,7 +85,421 @@
     <t>salesmanager149</t>
   </si>
   <si>
-    <t>salesmanager300</t>
+    <t>user2</t>
+  </si>
+  <si>
+    <t>user3</t>
+  </si>
+  <si>
+    <t>user4</t>
+  </si>
+  <si>
+    <t>user5</t>
+  </si>
+  <si>
+    <t>user6</t>
+  </si>
+  <si>
+    <t>user7</t>
+  </si>
+  <si>
+    <t>user8</t>
+  </si>
+  <si>
+    <t>user9</t>
+  </si>
+  <si>
+    <t>user10</t>
+  </si>
+  <si>
+    <t>user11</t>
+  </si>
+  <si>
+    <t>user12</t>
+  </si>
+  <si>
+    <t>user13</t>
+  </si>
+  <si>
+    <t>user14</t>
+  </si>
+  <si>
+    <t>user15</t>
+  </si>
+  <si>
+    <t>user16</t>
+  </si>
+  <si>
+    <t>user17</t>
+  </si>
+  <si>
+    <t>user18</t>
+  </si>
+  <si>
+    <t>user19</t>
+  </si>
+  <si>
+    <t>user20</t>
+  </si>
+  <si>
+    <t>user21</t>
+  </si>
+  <si>
+    <t>user22</t>
+  </si>
+  <si>
+    <t>user23</t>
+  </si>
+  <si>
+    <t>user24</t>
+  </si>
+  <si>
+    <t>user25</t>
+  </si>
+  <si>
+    <t>user26</t>
+  </si>
+  <si>
+    <t>user27</t>
+  </si>
+  <si>
+    <t>user28</t>
+  </si>
+  <si>
+    <t>user29</t>
+  </si>
+  <si>
+    <t>user30</t>
+  </si>
+  <si>
+    <t>user31</t>
+  </si>
+  <si>
+    <t>user33</t>
+  </si>
+  <si>
+    <t>user34</t>
+  </si>
+  <si>
+    <t>user35</t>
+  </si>
+  <si>
+    <t>user36</t>
+  </si>
+  <si>
+    <t>user37</t>
+  </si>
+  <si>
+    <t>user38</t>
+  </si>
+  <si>
+    <t>user39</t>
+  </si>
+  <si>
+    <t>user40</t>
+  </si>
+  <si>
+    <t>user41</t>
+  </si>
+  <si>
+    <t>user42</t>
+  </si>
+  <si>
+    <t>user43</t>
+  </si>
+  <si>
+    <t>user44</t>
+  </si>
+  <si>
+    <t>user45</t>
+  </si>
+  <si>
+    <t>user46</t>
+  </si>
+  <si>
+    <t>user47</t>
+  </si>
+  <si>
+    <t>user48</t>
+  </si>
+  <si>
+    <t>user49</t>
+  </si>
+  <si>
+    <t>user50</t>
+  </si>
+  <si>
+    <t>storemanager52</t>
+  </si>
+  <si>
+    <t>storemanager53</t>
+  </si>
+  <si>
+    <t>storemanager54</t>
+  </si>
+  <si>
+    <t>storemanager55</t>
+  </si>
+  <si>
+    <t>storemanager56</t>
+  </si>
+  <si>
+    <t>storemanager58</t>
+  </si>
+  <si>
+    <t>storemanager59</t>
+  </si>
+  <si>
+    <t>storemanager60</t>
+  </si>
+  <si>
+    <t>storemanager61</t>
+  </si>
+  <si>
+    <t>storemanager62</t>
+  </si>
+  <si>
+    <t>storemanager63</t>
+  </si>
+  <si>
+    <t>storemanager64</t>
+  </si>
+  <si>
+    <t>storemanager66</t>
+  </si>
+  <si>
+    <t>storemanager67</t>
+  </si>
+  <si>
+    <t>storemanager68</t>
+  </si>
+  <si>
+    <t>storemanager69</t>
+  </si>
+  <si>
+    <t>storemanager70</t>
+  </si>
+  <si>
+    <t>storemanager71</t>
+  </si>
+  <si>
+    <t>storemanager72</t>
+  </si>
+  <si>
+    <t>storemanager73</t>
+  </si>
+  <si>
+    <t>storemanager74</t>
+  </si>
+  <si>
+    <t>storemanager75</t>
+  </si>
+  <si>
+    <t>storemanager76</t>
+  </si>
+  <si>
+    <t>storemanager77</t>
+  </si>
+  <si>
+    <t>storemanager78</t>
+  </si>
+  <si>
+    <t>storemanager79</t>
+  </si>
+  <si>
+    <t>storemanager80</t>
+  </si>
+  <si>
+    <t>storemanager82</t>
+  </si>
+  <si>
+    <t>storemanager83</t>
+  </si>
+  <si>
+    <t>storemanager84</t>
+  </si>
+  <si>
+    <t>storemanager85</t>
+  </si>
+  <si>
+    <t>storemanager86</t>
+  </si>
+  <si>
+    <t>storemanager87</t>
+  </si>
+  <si>
+    <t>storemanager88</t>
+  </si>
+  <si>
+    <t>storemanager89</t>
+  </si>
+  <si>
+    <t>storemanager90</t>
+  </si>
+  <si>
+    <t>storemanager91</t>
+  </si>
+  <si>
+    <t>storemanager92</t>
+  </si>
+  <si>
+    <t>storemanager93</t>
+  </si>
+  <si>
+    <t>storemanager94</t>
+  </si>
+  <si>
+    <t>storemanager95</t>
+  </si>
+  <si>
+    <t>storemanager96</t>
+  </si>
+  <si>
+    <t>storemanager97</t>
+  </si>
+  <si>
+    <t>storemanager98</t>
+  </si>
+  <si>
+    <t>storemanager99</t>
+  </si>
+  <si>
+    <t>salesmanager102</t>
+  </si>
+  <si>
+    <t>salesmanager103</t>
+  </si>
+  <si>
+    <t>salesmanager104</t>
+  </si>
+  <si>
+    <t>salesmanager105</t>
+  </si>
+  <si>
+    <t>salesmanager106</t>
+  </si>
+  <si>
+    <t>salesmanager107</t>
+  </si>
+  <si>
+    <t>salesmanager108</t>
+  </si>
+  <si>
+    <t>salesmanager109</t>
+  </si>
+  <si>
+    <t>salesmanager110</t>
+  </si>
+  <si>
+    <t>salesmanager111</t>
+  </si>
+  <si>
+    <t>salesmanager112</t>
+  </si>
+  <si>
+    <t>salesmanager113</t>
+  </si>
+  <si>
+    <t>salesmanager114</t>
+  </si>
+  <si>
+    <t>salesmanager115</t>
+  </si>
+  <si>
+    <t>salesmanager116</t>
+  </si>
+  <si>
+    <t>salesmanager117</t>
+  </si>
+  <si>
+    <t>salesmanager118</t>
+  </si>
+  <si>
+    <t>salesmanager119</t>
+  </si>
+  <si>
+    <t>salesmanager120</t>
+  </si>
+  <si>
+    <t>salesmanager122</t>
+  </si>
+  <si>
+    <t>salesmanager123</t>
+  </si>
+  <si>
+    <t>salesmanager124</t>
+  </si>
+  <si>
+    <t>salesmanager125</t>
+  </si>
+  <si>
+    <t>salesmanager126</t>
+  </si>
+  <si>
+    <t>salesmanager127</t>
+  </si>
+  <si>
+    <t>salesmanager128</t>
+  </si>
+  <si>
+    <t>salesmanager129</t>
+  </si>
+  <si>
+    <t>salesmanager130</t>
+  </si>
+  <si>
+    <t>salesmanager131</t>
+  </si>
+  <si>
+    <t>salesmanager132</t>
+  </si>
+  <si>
+    <t>salesmanager133</t>
+  </si>
+  <si>
+    <t>salesmanager134</t>
+  </si>
+  <si>
+    <t>salesmanager135</t>
+  </si>
+  <si>
+    <t>salesmanager136</t>
+  </si>
+  <si>
+    <t>salesmanager137</t>
+  </si>
+  <si>
+    <t>salesmanager138</t>
+  </si>
+  <si>
+    <t>salesmanager139</t>
+  </si>
+  <si>
+    <t>salesmanager140</t>
+  </si>
+  <si>
+    <t>salesmanager141</t>
+  </si>
+  <si>
+    <t>salesmanager142</t>
+  </si>
+  <si>
+    <t>salesmanager143</t>
+  </si>
+  <si>
+    <t>salesmanager144</t>
+  </si>
+  <si>
+    <t>salesmanager145</t>
+  </si>
+  <si>
+    <t>salesmanager146</t>
+  </si>
+  <si>
+    <t>salesmanager148</t>
+  </si>
+  <si>
+    <t>salesmanager150</t>
   </si>
 </sst>
 </file>
@@ -110,8 +515,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -143,10 +547,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -461,10 +864,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F393E7B-4867-0241-ADCF-C3FB7C3D8FBD}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="212" zoomScaleNormal="212" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="212" zoomScaleNormal="212" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -492,10 +895,10 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
         <v>4</v>
@@ -503,49 +906,545 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>64</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>65</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>18</v>
+        <v>66</v>
+      </c>
+      <c r="C5" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" t="s">
+        <v>71</v>
+      </c>
+      <c r="C11" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" t="s">
+        <v>73</v>
+      </c>
+      <c r="C13" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" t="s">
+        <v>74</v>
+      </c>
+      <c r="C14" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" t="s">
+        <v>75</v>
+      </c>
+      <c r="C15" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" t="s">
         <v>9</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C16" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" t="s">
+        <v>76</v>
+      </c>
+      <c r="C17" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" t="s">
+        <v>77</v>
+      </c>
+      <c r="C18" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" t="s">
+        <v>78</v>
+      </c>
+      <c r="C19" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" t="s">
+        <v>79</v>
+      </c>
+      <c r="C20" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" t="s">
+        <v>80</v>
+      </c>
+      <c r="C21" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" t="s">
+        <v>81</v>
+      </c>
+      <c r="C22" t="s">
         <v>13</v>
       </c>
-      <c r="C6" t="s">
-        <v>19</v>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" t="s">
+        <v>82</v>
+      </c>
+      <c r="C23" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" t="s">
+        <v>83</v>
+      </c>
+      <c r="C24" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" t="s">
+        <v>84</v>
+      </c>
+      <c r="C25" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" t="s">
+        <v>85</v>
+      </c>
+      <c r="C26" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27" t="s">
+        <v>86</v>
+      </c>
+      <c r="C27" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28" t="s">
+        <v>87</v>
+      </c>
+      <c r="C28" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>42</v>
+      </c>
+      <c r="B29" t="s">
+        <v>88</v>
+      </c>
+      <c r="C29" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>43</v>
+      </c>
+      <c r="B30" t="s">
+        <v>89</v>
+      </c>
+      <c r="C30" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>44</v>
+      </c>
+      <c r="B31" t="s">
+        <v>90</v>
+      </c>
+      <c r="C31" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>45</v>
+      </c>
+      <c r="B32" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" t="s">
+        <v>91</v>
+      </c>
+      <c r="C33" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>46</v>
+      </c>
+      <c r="B34" t="s">
+        <v>92</v>
+      </c>
+      <c r="C34" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>47</v>
+      </c>
+      <c r="B35" t="s">
+        <v>93</v>
+      </c>
+      <c r="C35" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>48</v>
+      </c>
+      <c r="B36" t="s">
+        <v>94</v>
+      </c>
+      <c r="C36" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>49</v>
+      </c>
+      <c r="B37" t="s">
+        <v>95</v>
+      </c>
+      <c r="C37" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>50</v>
+      </c>
+      <c r="B38" t="s">
+        <v>96</v>
+      </c>
+      <c r="C38" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>51</v>
+      </c>
+      <c r="B39" t="s">
+        <v>97</v>
+      </c>
+      <c r="C39" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>52</v>
+      </c>
+      <c r="B40" t="s">
+        <v>98</v>
+      </c>
+      <c r="C40" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>53</v>
+      </c>
+      <c r="B41" t="s">
+        <v>99</v>
+      </c>
+      <c r="C41" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>54</v>
+      </c>
+      <c r="B42" t="s">
+        <v>100</v>
+      </c>
+      <c r="C42" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>55</v>
+      </c>
+      <c r="B43" t="s">
+        <v>101</v>
+      </c>
+      <c r="C43" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>56</v>
+      </c>
+      <c r="B44" t="s">
+        <v>102</v>
+      </c>
+      <c r="C44" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>57</v>
+      </c>
+      <c r="B45" t="s">
+        <v>103</v>
+      </c>
+      <c r="C45" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>58</v>
+      </c>
+      <c r="B46" t="s">
+        <v>104</v>
+      </c>
+      <c r="C46" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>59</v>
+      </c>
+      <c r="B47" t="s">
+        <v>105</v>
+      </c>
+      <c r="C47" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>60</v>
+      </c>
+      <c r="B48" t="s">
+        <v>106</v>
+      </c>
+      <c r="C48" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>61</v>
+      </c>
+      <c r="B49" t="s">
+        <v>107</v>
+      </c>
+      <c r="C49" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>62</v>
+      </c>
+      <c r="B50" t="s">
+        <v>108</v>
+      </c>
+      <c r="C50" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>63</v>
+      </c>
+      <c r="B51" t="s">
+        <v>10</v>
+      </c>
+      <c r="C51" t="s">
+        <v>154</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
finished (login and logout features)
</commit_message>
<xml_diff>
--- a/credentials.xlsx
+++ b/credentials.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/values/IdeaProjects/XFleet_Cucumber/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F8111DE-97D0-6D4F-9CF4-A85667ED8625}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D710EBF-717A-FD42-81A1-8BF631D286FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-56600" yWindow="-6800" windowWidth="27640" windowHeight="16940" xr2:uid="{AC3FA72D-1D93-084B-BC8B-B298B3374332}"/>
+    <workbookView xWindow="-28000" yWindow="-4460" windowWidth="27640" windowHeight="16940" xr2:uid="{AC3FA72D-1D93-084B-BC8B-B298B3374332}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -866,7 +866,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F393E7B-4867-0241-ADCF-C3FB7C3D8FBD}">
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="212" zoomScaleNormal="212" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="212" zoomScaleNormal="212" workbookViewId="0">
       <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>

</xml_diff>